<commit_message>
add disable property for IObject
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Comm/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/Comm/IObject.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uowou\Desktop\NFGameDemo\NoahFrame\_Out\NFDataCfg\Excel\Comm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uowou\Desktop\NFGameDemo\_Out\NFDataCfg\Excel\Comm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E71D43-D136-4A34-8852-9555DE02CB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02B0F6-0B58-4E8C-947F-96679787D221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="37636" windowHeight="20416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>object</t>
+  </si>
+  <si>
+    <t>Disable</t>
   </si>
 </sst>
 </file>
@@ -662,11 +665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -676,7 +679,7 @@
     <col min="5" max="5" width="9.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -713,8 +716,11 @@
       <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="M1" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1">
+    <row r="2" spans="1:13" s="2" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -751,8 +757,11 @@
       <c r="L2" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="M2" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:13" s="2" customFormat="1">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -789,8 +798,11 @@
       <c r="L3" s="10">
         <v>1</v>
       </c>
+      <c r="M3" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1">
+    <row r="4" spans="1:13" s="2" customFormat="1">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -827,8 +839,11 @@
       <c r="L4" s="10">
         <v>1</v>
       </c>
+      <c r="M4" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1">
+    <row r="5" spans="1:13" s="2" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -865,8 +880,11 @@
       <c r="L5" s="10">
         <v>0</v>
       </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1">
+    <row r="6" spans="1:13" s="2" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -903,8 +921,11 @@
       <c r="L6" s="3">
         <v>0</v>
       </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1">
+    <row r="7" spans="1:13" s="3" customFormat="1">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -941,8 +962,11 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1">
+    <row r="8" spans="1:13" s="3" customFormat="1">
       <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
@@ -979,8 +1003,11 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1">
+    <row r="9" spans="1:13" s="3" customFormat="1">
       <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
@@ -1017,8 +1044,11 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1">
+    <row r="10" spans="1:13" s="4" customFormat="1">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1031,11 +1061,12 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 I1:L1 A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 I2 B3:C3 F3:L6 F10:F1048576 I10:L1048576 B7:L9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 I1:M1 A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 I2 B3:C3 F3:M6 F10:F1048576 I10:M1048576 B7:M9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add connection status for object
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Comm/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/Comm/IObject.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28">
   <si>
     <t>Id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Disable</t>
+  </si>
+  <si>
+    <t>Connection</t>
   </si>
   <si>
     <t>Type</t>
@@ -102,10 +105,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -129,8 +132,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,6 +143,27 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,13 +177,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -167,6 +185,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -174,91 +208,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,6 +252,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -301,25 +304,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,31 +430,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,121 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,6 +610,21 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,6 +653,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -646,6 +673,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,30 +703,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -697,164 +711,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1291,12 +1294,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1304,9 +1307,10 @@
     <col min="1" max="2" width="10.4711538461538" customWidth="1"/>
     <col min="3" max="4" width="8.47115384615385" customWidth="1"/>
     <col min="5" max="5" width="9.47115384615385" customWidth="1"/>
+    <col min="15" max="15" width="12.0769230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:14">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1349,54 +1353,60 @@
       <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:14">
+    <row r="2" s="2" customFormat="1" spans="1:15">
       <c r="A2" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="O2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:14">
+    <row r="3" s="2" customFormat="1" spans="1:15">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -1435,12 +1445,15 @@
         <v>1</v>
       </c>
       <c r="N3" s="9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:14">
+    <row r="4" s="2" customFormat="1" spans="1:15">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -1481,10 +1494,13 @@
       <c r="N4" s="9">
         <v>1</v>
       </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:14">
+    <row r="5" s="2" customFormat="1" spans="1:15">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -1525,10 +1541,13 @@
       <c r="N5" s="9">
         <v>0</v>
       </c>
+      <c r="O5" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:14">
+    <row r="6" s="2" customFormat="1" spans="1:15">
       <c r="A6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -1569,10 +1588,13 @@
       <c r="N6" s="3">
         <v>0</v>
       </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:14">
+    <row r="7" s="3" customFormat="1" ht="17" spans="1:15">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1613,10 +1635,13 @@
       <c r="N7" s="3">
         <v>0</v>
       </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:14">
+    <row r="8" s="3" customFormat="1" ht="17" spans="1:15">
       <c r="A8" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1657,10 +1682,13 @@
       <c r="N8" s="3">
         <v>0</v>
       </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:14">
+    <row r="9" s="3" customFormat="1" ht="17" spans="1:15">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1701,10 +1729,13 @@
       <c r="N9" s="3">
         <v>0</v>
       </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="17.55" spans="1:14">
+    <row r="10" s="4" customFormat="1" ht="17.55" spans="1:15">
       <c r="A10" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1716,11 +1747,12 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 J1:N1 A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 J2 B3:C3 J3 K3 L3:N3 J4 K4 L4:N4 F10:F1048576 I3:I6 I7:I9 F3:H6 B7:H9 J10:N1048576 J7:N9 J5:N6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 J1:N1 O1 A7:A9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 J2 B3:C3 J3 K3 L3:M3 N3 O3 J4 K4 L4:M4 N4 O4 F10:F1048576 I3:I6 I7:I9 O5:O6 O7:O9 O10:O1048576 F3:H6 B7:H9 J10:N1048576 J7:N9 J5:N6">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>